<commit_message>
reorganize components, add moment.js, check pages at interval
</commit_message>
<xml_diff>
--- a/Page checker/Page checker/doc/doc.xlsx
+++ b/Page checker/Page checker/doc/doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,47 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Validated</t>
-  </si>
-  <si>
-    <t>Checksum</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TODO</t>
   </si>
   <si>
-    <t>Check now</t>
-  </si>
-  <si>
-    <t>Polling Interval</t>
-  </si>
-  <si>
-    <t>12 hours</t>
-  </si>
-  <si>
-    <t>Last time</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
     <t>"Add current Page" button</t>
   </si>
   <si>
     <t>"Delete" button</t>
   </si>
   <si>
-    <t>"Schedule period" button</t>
-  </si>
-  <si>
     <t>Polling interval</t>
   </si>
   <si>
@@ -69,24 +39,32 @@
     <t>Array selection : change look : first, last,use coutn, specific index</t>
   </si>
   <si>
-    <t>Bootstrap (npm)</t>
+    <t>take a look at Bootstrap (npm)</t>
+  </si>
+  <si>
+    <t>O first element</t>
+  </si>
+  <si>
+    <t>O Last element</t>
+  </si>
+  <si>
+    <t>O use count as result</t>
+  </si>
+  <si>
+    <t>O Specific index</t>
+  </si>
+  <si>
+    <t>checksum undefined after extension load. Not saved ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,21 +81,24 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,55 +107,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -194,107 +156,40 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>134416</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>48042</xdr:rowOff>
+      <xdr:colOff>115323</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>134007</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="514350" y="295275"/>
-          <a:ext cx="7640116" cy="2991267"/>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="7325748" cy="4706007"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2314575" y="704850"/>
-          <a:ext cx="1219200" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Add current Page</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -343,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,10 +270,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +304,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,106 +479,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:Z24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D6:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="13:26">
       <c r="M6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="13:26">
+      <c r="N7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="13:26">
+      <c r="N8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" s="1"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="13:26">
+      <c r="N9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N7" t="s">
+    <row r="10" spans="13:26">
+      <c r="N10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="13:26">
+      <c r="N11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="13:26">
+      <c r="N12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="13:26">
+      <c r="N14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="13:26">
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" ht="15.75" thickBot="1">
+      <c r="D33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N8" t="s">
+    <row r="34" spans="4:6" ht="15.75" thickBot="1">
+      <c r="D34" t="s">
         <v>11</v>
       </c>
-      <c r="U8" s="2"/>
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="13:26" x14ac:dyDescent="0.25">
-      <c r="N15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="6">
-        <v>42745.560416666667</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>123456</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="F34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -695,24 +572,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
collapse all, expand all
</commit_message>
<xml_diff>
--- a/Page checker/Page checker/doc/doc.xlsx
+++ b/Page checker/Page checker/doc/doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>bower : tracetool.js</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Add export button</t>
-  </si>
-  <si>
-    <t>Mimimize all, collapse all</t>
-  </si>
-  <si>
-    <t>Save minimized state by scanner (reopen the popup)</t>
   </si>
   <si>
     <t>Manual check : don't unvalidate</t>
@@ -461,7 +455,7 @@
   <dimension ref="F6:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +470,7 @@
   <sheetData>
     <row r="6" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="14:17" x14ac:dyDescent="0.25">
@@ -484,11 +478,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N8" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="9" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N9" t="s">
         <v>8</v>
@@ -497,11 +486,6 @@
     <row r="10" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N10" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="14:17" x14ac:dyDescent="0.25">

</xml_diff>